<commit_message>
update bulk upload files
</commit_message>
<xml_diff>
--- a/e2e-tests/data/bulk_booking_upload.xlsx
+++ b/e2e-tests/data/bulk_booking_upload.xlsx
@@ -877,6 +877,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -897,9 +900,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="289">
@@ -1469,7 +1469,7 @@
   <dimension ref="A1:AZ4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1527,56 +1527,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
-      <c r="W1" s="20" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20"/>
+      <c r="W1" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="21" t="s">
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="22" t="s">
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="22"/>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="16" t="s">
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="23"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="23"/>
+      <c r="AQ1" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="16"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="16" t="s">
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="AW1" s="16"/>
-      <c r="AX1" s="16" t="s">
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="AY1" s="16"/>
+      <c r="AY1" s="17"/>
       <c r="AZ1" s="7" t="s">
         <v>106</v>
       </c>
@@ -1657,7 +1657,7 @@
       <c r="Y2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="23" t="s">
+      <c r="Z2" s="16" t="s">
         <v>20</v>
       </c>
       <c r="AA2" s="13" t="s">
@@ -1750,10 +1750,10 @@
         <v>109</v>
       </c>
       <c r="D3" s="3">
-        <v>43081.416666666664</v>
+        <v>46733.416666666664</v>
       </c>
       <c r="E3" s="3">
-        <v>43081.458333333336</v>
+        <v>46733.458333333336</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>28</v>
@@ -1893,10 +1893,10 @@
         <v>109</v>
       </c>
       <c r="D4" s="3">
-        <v>43243.5</v>
+        <v>46896.5</v>
       </c>
       <c r="E4" s="3">
-        <v>43243.583333333336</v>
+        <v>46896.583333333336</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
updated spreadsheets to new format
</commit_message>
<xml_diff>
--- a/e2e-tests/data/bulk_booking_upload.xlsx
+++ b/e2e-tests/data/bulk_booking_upload.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rasta/Projects/Curve/auslan/booking-system-api/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B1F0D8-4DD8-9440-B788-9ED04E5F5F75}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="8260" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="51200" yWindow="8260" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,13 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="123">
-  <si>
-    <t>Start date &amp; time</t>
-  </si>
-  <si>
-    <t>End date &amp; time</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="129">
   <si>
     <t>Specific location</t>
   </si>
@@ -41,36 +36,6 @@
     <t>Unit number</t>
   </si>
   <si>
-    <t>Street number</t>
-  </si>
-  <si>
-    <t>Street name</t>
-  </si>
-  <si>
-    <t>Suburb</t>
-  </si>
-  <si>
-    <t>Post code</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Nature of appointment</t>
-  </si>
-  <si>
-    <t>What will be discussed</t>
-  </si>
-  <si>
-    <t>Who requested this meeting first name</t>
-  </si>
-  <si>
-    <t>Who requested this meeting last name</t>
-  </si>
-  <si>
-    <t>Number of people attending</t>
-  </si>
-  <si>
     <t>Parking availability</t>
   </si>
   <si>
@@ -80,329 +45,383 @@
     <t>Special instructions</t>
   </si>
   <si>
-    <t>Contact first name</t>
-  </si>
-  <si>
-    <t>Contact last name</t>
-  </si>
-  <si>
-    <t>Contact email</t>
-  </si>
-  <si>
     <t>Contact mobile</t>
   </si>
   <si>
+    <t>Deaf person's mobile</t>
+  </si>
+  <si>
+    <t>External reference number</t>
+  </si>
+  <si>
+    <t>Level 25 Room 2</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>Medical</t>
+  </si>
+  <si>
+    <t>Audiology</t>
+  </si>
+  <si>
+    <t>Gideon</t>
+  </si>
+  <si>
+    <t>Malick</t>
+  </si>
+  <si>
+    <t>2 bays</t>
+  </si>
+  <si>
+    <t>Bring a book</t>
+  </si>
+  <si>
+    <t>Whatever</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Couslon</t>
+  </si>
+  <si>
+    <t>agent@curvetomorrow.com.au</t>
+  </si>
+  <si>
+    <t>0409 021 703</t>
+  </si>
+  <si>
+    <t>Jemma</t>
+  </si>
+  <si>
+    <t>Ward</t>
+  </si>
+  <si>
+    <t>jemma@ward.com</t>
+  </si>
+  <si>
+    <t>0400 123 456</t>
+  </si>
+  <si>
+    <t>ACCADACCA</t>
+  </si>
+  <si>
+    <t>Thijs</t>
+  </si>
+  <si>
+    <t>Sondag</t>
+  </si>
+  <si>
+    <t>thijs@curvetomorrow.com.au</t>
+  </si>
+  <si>
+    <t>0422 123 456</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Ellos Street</t>
+  </si>
+  <si>
+    <t>NSW</t>
+  </si>
+  <si>
+    <t>Hyde Park</t>
+  </si>
+  <si>
+    <t>121B</t>
+  </si>
+  <si>
+    <t>Ellis St</t>
+  </si>
+  <si>
+    <t>Matheson Rd</t>
+  </si>
+  <si>
+    <t>Applecross</t>
+  </si>
+  <si>
+    <t>VIC</t>
+  </si>
+  <si>
+    <t>Point Cook</t>
+  </si>
+  <si>
+    <t>Police</t>
+  </si>
+  <si>
+    <t>Arrest</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Don't be late</t>
+  </si>
+  <si>
+    <t>Nada</t>
+  </si>
+  <si>
+    <t>Rebecca</t>
+  </si>
+  <si>
+    <t>Fitzgerald</t>
+  </si>
+  <si>
+    <t>bec@gmail.com</t>
+  </si>
+  <si>
+    <t>0432 123 433</t>
+  </si>
+  <si>
+    <t>Skye</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>skye@gmail.com</t>
+  </si>
+  <si>
+    <t>0456 732 343</t>
+  </si>
+  <si>
+    <t>3132-232-233</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Warren</t>
+  </si>
+  <si>
+    <t>george@gmail.com</t>
+  </si>
+  <si>
+    <t>09 3322 1123</t>
+  </si>
+  <si>
+    <t>Kintail Rd</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>TAS</t>
+  </si>
+  <si>
+    <t>Hobart</t>
+  </si>
+  <si>
+    <t>Booking Location</t>
+  </si>
+  <si>
+    <t>Contact info</t>
+  </si>
+  <si>
+    <t>Deaf person's details</t>
+  </si>
+  <si>
+    <t>Billing Account</t>
+  </si>
+  <si>
+    <t>alana@auslan.com.au</t>
+  </si>
+  <si>
+    <t>onsite</t>
+  </si>
+  <si>
+    <t>vri</t>
+  </si>
+  <si>
+    <t>Captioning</t>
+  </si>
+  <si>
+    <t>Tech Contact First Name</t>
+  </si>
+  <si>
+    <t>Tech Contact Phone Number</t>
+  </si>
+  <si>
+    <t>Tech Contact Email</t>
+  </si>
+  <si>
+    <t>Tech Contact Last Name</t>
+  </si>
+  <si>
+    <t>Tech Platorm</t>
+  </si>
+  <si>
+    <t>Login ID/Link</t>
+  </si>
+  <si>
+    <t>Audio Source</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>How would you like to receive notes?</t>
+  </si>
+  <si>
+    <t>Who will initiate call?</t>
+  </si>
+  <si>
+    <t>Note Taking</t>
+  </si>
+  <si>
+    <t>VRI</t>
+  </si>
+  <si>
+    <t>Captioning or VRI</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Turtle</t>
+  </si>
+  <si>
+    <t>adam@curve.com.au</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>Mac</t>
+  </si>
+  <si>
+    <t>aturtle</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>0400 000 000</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>bump</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>UR NUMBER</t>
+  </si>
+  <si>
+    <t>NDIS ID</t>
+  </si>
+  <si>
+    <t>UR123</t>
+  </si>
+  <si>
+    <t>UR453</t>
+  </si>
+  <si>
+    <t>NDIS12</t>
+  </si>
+  <si>
+    <t>NDIS55</t>
+  </si>
+  <si>
     <t>EAF-id</t>
   </si>
   <si>
-    <t>Deaf person's first name</t>
-  </si>
-  <si>
-    <t>Deaf person's last name</t>
-  </si>
-  <si>
-    <t>Deaf person's email</t>
-  </si>
-  <si>
-    <t>Deaf person's mobile</t>
-  </si>
-  <si>
-    <t>External reference number</t>
-  </si>
-  <si>
-    <t>Contact number</t>
-  </si>
-  <si>
-    <t>Level 25 Room 2</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t>Medical</t>
-  </si>
-  <si>
-    <t>Audiology</t>
-  </si>
-  <si>
-    <t>Gideon</t>
-  </si>
-  <si>
-    <t>Malick</t>
-  </si>
-  <si>
-    <t>2 bays</t>
-  </si>
-  <si>
-    <t>Bring a book</t>
-  </si>
-  <si>
-    <t>Whatever</t>
-  </si>
-  <si>
-    <t>Agent</t>
-  </si>
-  <si>
-    <t>Couslon</t>
-  </si>
-  <si>
-    <t>agent@curvetomorrow.com.au</t>
-  </si>
-  <si>
-    <t>0409 021 703</t>
-  </si>
-  <si>
-    <t>Jemma</t>
-  </si>
-  <si>
-    <t>Ward</t>
-  </si>
-  <si>
-    <t>jemma@ward.com</t>
-  </si>
-  <si>
-    <t>0400 123 456</t>
-  </si>
-  <si>
-    <t>ACCADACCA</t>
-  </si>
-  <si>
-    <t>Thijs</t>
-  </si>
-  <si>
-    <t>Sondag</t>
-  </si>
-  <si>
-    <t>thijs@curvetomorrow.com.au</t>
-  </si>
-  <si>
-    <t>0422 123 456</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Ellos Street</t>
-  </si>
-  <si>
-    <t>NSW</t>
-  </si>
-  <si>
-    <t>Hyde Park</t>
-  </si>
-  <si>
-    <t>121B</t>
-  </si>
-  <si>
-    <t>Ellis St</t>
-  </si>
-  <si>
-    <t>Matheson Rd</t>
-  </si>
-  <si>
-    <t>Applecross</t>
-  </si>
-  <si>
-    <t>VIC</t>
-  </si>
-  <si>
-    <t>Point Cook</t>
-  </si>
-  <si>
-    <t>Police</t>
-  </si>
-  <si>
-    <t>Arrest</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Don't be late</t>
-  </si>
-  <si>
-    <t>Nada</t>
-  </si>
-  <si>
-    <t>Rebecca</t>
-  </si>
-  <si>
-    <t>Fitzgerald</t>
-  </si>
-  <si>
-    <t>bec@gmail.com</t>
-  </si>
-  <si>
-    <t>0432 123 433</t>
-  </si>
-  <si>
-    <t>Skye</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>skye@gmail.com</t>
-  </si>
-  <si>
-    <t>0456 732 343</t>
-  </si>
-  <si>
-    <t>3132-232-233</t>
-  </si>
-  <si>
-    <t>George</t>
-  </si>
-  <si>
-    <t>Warren</t>
-  </si>
-  <si>
-    <t>george@gmail.com</t>
-  </si>
-  <si>
-    <t>09 3322 1123</t>
-  </si>
-  <si>
-    <t>Kintail Rd</t>
-  </si>
-  <si>
-    <t>Sydney</t>
-  </si>
-  <si>
-    <t>TAS</t>
-  </si>
-  <si>
-    <t>Hobart</t>
-  </si>
-  <si>
-    <t>Booking Location</t>
-  </si>
-  <si>
-    <t>Contact info</t>
-  </si>
-  <si>
-    <t>Deaf person's details</t>
-  </si>
-  <si>
-    <t>Billing Account</t>
-  </si>
-  <si>
-    <t>alana@auslan.com.au</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Kind of service (onsite, vri)</t>
-  </si>
-  <si>
-    <t>onsite</t>
-  </si>
-  <si>
-    <t>vri</t>
-  </si>
-  <si>
-    <t>Number of interpreters needed</t>
-  </si>
-  <si>
-    <t>Type of Interpreting (ASL, Auslan, BSL, Captioning, Deaf Blind, Deaf, Indigineous Sign, ISL, Note Taking, Platform, Signed English, Tactile, Visual Frame)</t>
-  </si>
-  <si>
-    <t>Captioning</t>
-  </si>
-  <si>
-    <t>Tech Contact First Name</t>
-  </si>
-  <si>
-    <t>Tech Contact Phone Number</t>
-  </si>
-  <si>
-    <t>Tech Contact Email</t>
-  </si>
-  <si>
-    <t>Tech Contact Last Name</t>
-  </si>
-  <si>
-    <t>Tech Platorm</t>
-  </si>
-  <si>
-    <t>Login ID/Link</t>
-  </si>
-  <si>
-    <t>Audio Source</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
-    <t>How would you like to receive notes?</t>
-  </si>
-  <si>
-    <t>Who will initiate call?</t>
-  </si>
-  <si>
-    <t>Note Taking</t>
-  </si>
-  <si>
-    <t>VRI</t>
-  </si>
-  <si>
-    <t>Captioning or VRI</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>Turtle</t>
-  </si>
-  <si>
-    <t>adam@curve.com.au</t>
-  </si>
-  <si>
-    <t>Speaker</t>
-  </si>
-  <si>
-    <t>Mac</t>
-  </si>
-  <si>
-    <t>aturtle</t>
-  </si>
-  <si>
-    <t>PDF</t>
-  </si>
-  <si>
-    <t>0400 000 000</t>
-  </si>
-  <si>
-    <t>Windows</t>
-  </si>
-  <si>
-    <t>bump</t>
-  </si>
-  <si>
-    <t>iPhone</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Linked (Y/N) - Set first row only</t>
+    <t>Email*</t>
+  </si>
+  <si>
+    <t>Kind of service (onsite, vri)*</t>
+  </si>
+  <si>
+    <t>Linked (Y/N) - Set first row only*</t>
+  </si>
+  <si>
+    <t>Start date &amp; time*</t>
+  </si>
+  <si>
+    <t>End date &amp; time*</t>
+  </si>
+  <si>
+    <t>Street number*</t>
+  </si>
+  <si>
+    <t>Street name*</t>
+  </si>
+  <si>
+    <t>Suburb*</t>
+  </si>
+  <si>
+    <t>Post code*</t>
+  </si>
+  <si>
+    <t>State*</t>
+  </si>
+  <si>
+    <t>Nature of appointment*</t>
+  </si>
+  <si>
+    <t>What will be discussed*</t>
+  </si>
+  <si>
+    <t>Who requested this meeting first name*</t>
+  </si>
+  <si>
+    <t>Who requested this meeting last name*</t>
+  </si>
+  <si>
+    <t>Number of people attending*</t>
+  </si>
+  <si>
+    <t>Number of interpreters needed*</t>
+  </si>
+  <si>
+    <t>Type of Interpreting (ASL, Auslan, BSL, Captioning, Deaf, Indigineous Sign, ISL, Note Taking, Platform, Signed English, Tactile, Visual Frame)*</t>
+  </si>
+  <si>
+    <t>Contact first name*</t>
+  </si>
+  <si>
+    <t>Contact last name*</t>
+  </si>
+  <si>
+    <t>Contact email*</t>
+  </si>
+  <si>
+    <t>Deaf person's first name*</t>
+  </si>
+  <si>
+    <t>Deaf person's last name*</t>
+  </si>
+  <si>
+    <t>Deaf person's email*</t>
+  </si>
+  <si>
+    <t>Contact number*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -446,8 +465,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,8 +518,41 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -546,8 +619,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="289">
+  <cellStyleXfs count="292">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -837,8 +934,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -852,33 +952,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -895,14 +968,51 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="289" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="290" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="291" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="291" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="289" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="289" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="290" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="291" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="289" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="289">
+  <cellStyles count="292">
+    <cellStyle name="Bad" xfId="290" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1118,6 +1228,7 @@
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="289" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1191,6 +1302,7 @@
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="291" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1198,6 +1310,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1465,11 +1580,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="268" zoomScaleNormal="268" workbookViewId="0">
+      <selection activeCell="S2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1500,254 +1615,263 @@
     <col min="24" max="24" width="14.5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="12.1640625" customWidth="1"/>
+    <col min="29" max="29" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="21" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="21" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="F1" s="18" t="s">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="F1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="11"/>
+      <c r="W1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="13"/>
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="13"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
-      <c r="W1" s="21" t="s">
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" s="26" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB2" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC2" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD2" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE2" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="AF2" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH2" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI2" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ2" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK2" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="AL2" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO2" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="AP2" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="AQ2" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="AR2" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="AS2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT2" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU2" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV2" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="AW2" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX2" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY2" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ2" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA2" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB2" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="23"/>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
-      <c r="AO1" s="23"/>
-      <c r="AP1" s="23"/>
-      <c r="AQ1" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR1" s="17"/>
-      <c r="AS1" s="17"/>
-      <c r="AT1" s="17"/>
-      <c r="AU1" s="17"/>
-      <c r="AV1" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="AW1" s="17"/>
-      <c r="AX1" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="AY1" s="17"/>
-      <c r="AZ1" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52" s="15" customFormat="1" ht="65" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z2" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF2" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI2" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="AK2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="AM2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="AO2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AP2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="AQ2" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AS2" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="AT2" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AU2" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AV2" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="AW2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="AX2" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AY2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AZ2" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D3" s="3">
         <v>46733.416666666664</v>
@@ -1756,37 +1880,37 @@
         <v>46733.458333333336</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="H3" s="1">
         <v>34</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="K3" s="1">
         <v>6153</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="Q3" s="1">
         <v>3</v>
@@ -1795,102 +1919,108 @@
         <v>2</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA3" s="6">
+        <v>21</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC3" s="6">
         <v>123564</v>
       </c>
-      <c r="AB3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>44</v>
+      <c r="AD3" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL3" s="1">
+        <v>29</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN3" s="1">
         <v>10</v>
       </c>
-      <c r="AM3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AO3" s="1">
+      <c r="AO3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ3" s="1">
         <v>2000</v>
       </c>
-      <c r="AP3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>118</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>119</v>
+      <c r="AR3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="AX3" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="AY3" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="AZ3" t="s">
-        <v>116</v>
+        <v>96</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="D4" s="3">
         <v>46896.5</v>
@@ -1899,37 +2029,37 @@
         <v>46896.583333333336</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="H4" s="1">
         <v>23</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="K4" s="1">
         <v>3030</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
@@ -1938,116 +2068,122 @@
         <v>5</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA4" s="1">
+        <v>50</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC4" s="1">
         <v>987675</v>
       </c>
-      <c r="AB4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>73</v>
+      <c r="AD4" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>78</v>
+        <v>55</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK4" s="1">
+        <v>57</v>
+      </c>
+      <c r="AK4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM4" s="1">
         <v>54</v>
       </c>
-      <c r="AL4" s="1">
+      <c r="AN4" s="1">
         <v>1245</v>
       </c>
-      <c r="AM4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO4" s="1">
+      <c r="AO4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ4" s="1">
         <v>4323</v>
       </c>
-      <c r="AP4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="AR4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AS4" s="4" t="s">
-        <v>112</v>
+        <v>62</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AU4" s="1" t="s">
-        <v>113</v>
+        <v>87</v>
+      </c>
+      <c r="AU4" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="AV4" s="1" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="AW4" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AX4" s="1"/>
-      <c r="AY4" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="AV1:AW1"/>
     <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="AZ1:BA1"/>
     <mergeCell ref="F1:L1"/>
     <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="AA1:AE1"/>
-    <mergeCell ref="AF1:AP1"/>
-    <mergeCell ref="AQ1:AU1"/>
+    <mergeCell ref="AH1:AR1"/>
+    <mergeCell ref="AS1:AW1"/>
+    <mergeCell ref="AA1:AG1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="Y4" r:id="rId1"/>
-    <hyperlink ref="AD4" r:id="rId2"/>
-    <hyperlink ref="AI4" r:id="rId3"/>
-    <hyperlink ref="AS4" r:id="rId4"/>
+    <hyperlink ref="Y4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="AF4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="AK4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="AU4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>